<commit_message>
Update with real time TCS
</commit_message>
<xml_diff>
--- a/TestData/LoginTestData.xlsx
+++ b/TestData/LoginTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation\New folder\DataDrivenFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation\DataDrivenFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A010BEC-9CB2-4915-9FB3-2F4C6B9A0F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044E0206-8DEB-4F72-A37E-DD6227E8846A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="LoginData" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">LoginData!$F$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">LoginData!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t xml:space="preserve">Project </t>
   </si>
@@ -45,10 +45,31 @@
     <t>Expected_Result</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Actual_Result</t>
+    <t>Swag Labs</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>"secret_sauce"</t>
+  </si>
+  <si>
+    <t>Username and password do not match any user in this service</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
   </si>
 </sst>
 </file>
@@ -117,14 +138,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Monospace"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -150,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -173,20 +195,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -206,16 +220,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -224,8 +232,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,31 +618,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK1"/>
+  <dimension ref="A1:AMI5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="9" customWidth="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.5703125" style="1"/>
-    <col min="10" max="10" width="29.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="1" customWidth="1"/>
-    <col min="14" max="1026" width="11.5703125" style="1"/>
-    <col min="1027" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="58.140625" style="10" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="1" customWidth="1"/>
+    <col min="12" max="1024" width="11.5703125" style="1"/>
+    <col min="1025" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9 1025:1025" s="9" customFormat="1" ht="19.5" customHeight="1">
+    <row r="1" spans="1:1023" s="7" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -646,16 +656,83 @@
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="4"/>
+      <c r="AMI1" s="8"/>
+    </row>
+    <row r="2" spans="1:1023">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="AMK1" s="10"/>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1023">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1023">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1023">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3595FCAC-449A-4474-89AC-DAD0C26F6E39}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{5C4FA15D-B3FD-4930-B32D-A73787B70938}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{D8F2B0F8-1696-4A57-8EDC-2BF6F0735627}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>